<commit_message>
Manage to create Final sheet if is not already.
</commit_message>
<xml_diff>
--- a/ExcelWriter/ExcelWriter/wwwroot/TestReport.xlsx
+++ b/ExcelWriter/ExcelWriter/wwwroot/TestReport.xlsx
@@ -9,8 +9,8 @@
   </bookViews>
   <sheets>
     <sheet name="F 20.04" sheetId="1" r:id="rId2"/>
-    <sheet name="Final" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Final" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcMode="auto" fullCalcOnLoad="0" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001" fullPrecision="1" calcCompleted="0" calcOnSave="0" concurrentCalc="0" forceFullCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t xml:space="preserve">20. Geographical breakdown</t>
   </si>
@@ -561,16 +561,16 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.14" style="0" customWidth="1"/>
+    <col min="1" max="1" width="9.13" style="0" customWidth="1"/>
     <col min="2" max="2" width="71.14" style="0" customWidth="1"/>
-    <col min="3" max="3" width="9.14" style="0" customWidth="1"/>
+    <col min="3" max="3" width="9.13" style="0" customWidth="1"/>
     <col min="4" max="4" width="48.57" style="0" customWidth="1"/>
     <col min="5" max="5" width="22.7" style="0" customWidth="1"/>
     <col min="6" max="6" width="16" style="0" customWidth="1"/>
     <col min="7" max="7" width="15.71" style="0" customWidth="1"/>
-    <col min="8" max="9" width="9.14" style="0" customWidth="1"/>
+    <col min="8" max="9" width="9.13" style="0" customWidth="1"/>
     <col min="10" max="10" width="24.71" style="0" customWidth="1"/>
     <col min="11" max="11" width="89.57" style="0" customWidth="1"/>
   </cols>
@@ -829,278 +829,14 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.14" style="0" customWidth="1"/>
-    <col min="2" max="2" width="71.14" style="0" customWidth="1"/>
-    <col min="3" max="3" width="9.14" style="0" customWidth="1"/>
-    <col min="4" max="4" width="48.57" style="0" customWidth="1"/>
-    <col min="5" max="5" width="22.7" style="0" customWidth="1"/>
-    <col min="6" max="6" width="14.15" style="0" customWidth="1"/>
-    <col min="7" max="7" width="17.71" style="0" customWidth="1"/>
-    <col min="8" max="8" width="9.14" style="0" customWidth="1"/>
-    <col min="9" max="9" width="8.29" style="0" customWidth="1"/>
-    <col min="10" max="10" width="24.71" style="0" customWidth="1"/>
-    <col min="11" max="11" width="89.57" style="0" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="15">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" ht="15">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" ht="15">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-    </row>
-    <row r="4" ht="15">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="1"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" ht="15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" ht="52.5">
-      <c r="A8" s="13"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" ht="31.5">
-      <c r="A9" s="13"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" ht="15">
-      <c r="A10" s="13"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" ht="20.45">
-      <c r="A11" s="13"/>
-      <c r="B11" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-    </row>
-    <row r="12" ht="30.1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-  </mergeCells>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15"/>
+  <sheetData/>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1116,17 +852,279 @@
   <sheetPr>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView showOutlineSymbols="1" defaultGridColor="1" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.13" style="0" customWidth="1"/>
+    <col min="2" max="2" width="71.14" style="0" customWidth="1"/>
+    <col min="3" max="3" width="9.13" style="0" customWidth="1"/>
+    <col min="4" max="4" width="48.57" style="0" customWidth="1"/>
+    <col min="5" max="5" width="22.7" style="0" customWidth="1"/>
+    <col min="6" max="6" width="16" style="0" customWidth="1"/>
+    <col min="7" max="7" width="15.71" style="0" customWidth="1"/>
+    <col min="8" max="9" width="9.13" style="0" customWidth="1"/>
+    <col min="10" max="10" width="24.71" style="0" customWidth="1"/>
+    <col min="11" max="11" width="89.57" style="0" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" ht="15">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" ht="15">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" ht="15">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" ht="64.5">
+      <c r="A5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" ht="15">
+      <c r="A6" s="1"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" ht="63">
+      <c r="A8" s="13"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" ht="63">
+      <c r="A9" s="13"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" ht="15">
+      <c r="A10" s="13"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" ht="21">
+      <c r="A11" s="13"/>
+      <c r="B11" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
+    </row>
+    <row r="12" ht="42">
+      <c r="A12" s="13"/>
+      <c r="B12" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="33"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+  </mergeCells>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader/>
     <oddFooter/>

</xml_diff>